<commit_message>
seed 이미지 경로 정리, fertilizer 리소스 추가. WPUserDataManager 버그 수정.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Fertilizer.xlsx
+++ b/Assets/StreamingAssets/Fertilizer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProject\WWWProject\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CD689C-D41E-48DA-BDED-F5F112D06036}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1002F4-A62B-4C65-A74F-4F399164FD46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5925" xr2:uid="{6CE15BC7-748E-45F8-AC45-97F3E40DA475}"/>
   </bookViews>
@@ -200,10 +200,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>fertilizer_Hen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>fertilizer_Duck</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -233,6 +229,10 @@
   </si>
   <si>
     <t>fertilizer_Napal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fertilizer_Chick</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -600,7 +600,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -723,7 +723,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -749,7 +749,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
@@ -775,7 +775,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
@@ -801,7 +801,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -827,7 +827,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -853,7 +853,7 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
@@ -879,7 +879,7 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
@@ -905,7 +905,7 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
         <v>23</v>
@@ -931,7 +931,7 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
         <v>23</v>

</xml_diff>